<commit_message>
formatted xls as table
</commit_message>
<xml_diff>
--- a/list_clus_data.xlsx
+++ b/list_clus_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="110">
   <si>
     <t>Roads</t>
   </si>
@@ -395,12 +395,6 @@
   </si>
   <si>
     <t>In postgres db?</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>mike here just testing github</t>
   </si>
 </sst>
 </file>
@@ -838,7 +832,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,12 +1651,6 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>110</v>
-      </c>
-      <c r="B32" t="s">
-        <v>111</v>
-      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="G32" s="1"/>

</xml_diff>

<commit_message>
minor edits to updates on postgres side
</commit_message>
<xml_diff>
--- a/list_clus_data.xlsx
+++ b/list_clus_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="24920" windowHeight="11020"/>
+    <workbookView xWindow="120" yWindow="140" windowWidth="24920" windowHeight="10960"/>
   </bookViews>
   <sheets>
     <sheet name="Table_Info" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="193">
   <si>
     <t>Roads</t>
   </si>
@@ -379,9 +379,6 @@
     <t>Forest Tenure</t>
   </si>
   <si>
-    <t>Administrative bounaries of Timber Supply Areas</t>
-  </si>
-  <si>
     <t>ogr2ogr -f PostgreSQL PG:"dbname=clus port = 5432 user=postgres" \\spatialfiles.bcgov\Work\srm\bcce\shared\data_library\roads\2017\BC_CE_IntegratedRoads_2017_v1_20170214.gdb "integrated_roads" -overwrite -progress --config PG_USE_COPY YES</t>
   </si>
   <si>
@@ -506,9 +503,6 @@
   </si>
   <si>
     <t>Downloaded; need to add to clus postgres db</t>
-  </si>
-  <si>
-    <t>study_area_caribou_herd_dissolve</t>
   </si>
   <si>
     <t xml:space="preserve">ogr2ogr -f PostgreSQL PG:"dbname=clus port = 5432 user=postgres" \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\study_areas\clus_study_areas.gdb "study_area_caribou_herd_dissolve" -lco SCHEMA=public -overwrite -progress --config PG_USE_COPY YES  </t>
@@ -624,6 +618,44 @@
   </si>
   <si>
     <t>...clus\R\caribou_protected_area\01_caribou_protected_areas_download.R</t>
+  </si>
+  <si>
+    <t>Administrative boundaries of Timber Supply Areas. WHSE_ADMIN_BOUNDARIES.FADM_TSA</t>
+  </si>
+  <si>
+    <t>Watercourses from TRIM enhanced base map</t>
+  </si>
+  <si>
+    <t>public.study_area_caribou_herd_dissolve</t>
+  </si>
+  <si>
+    <t>raster2pgsql -s 4326 -d -I -C -M -R C:\Users\KLOCHHEA\Downloads\mat_1961_1990.tif -t 100x100 public.mat_1961_1990 | psql -d clus</t>
+  </si>
+  <si>
+    <t>public.mat_1961_1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Postgresql can't store attribute table of a raster --well it can but it very messy as each unique value becomes a band and the band is then labeled by its atttribute name. Two work arounds i) keep </t>
+  </si>
+  <si>
+    <t xml:space="preserve">categorical data (i.e., bec zones) as vector data. If the categorical data is a raster - then vectorize it - all spatial query in R can accommodate these differences in geometry types or ii) map the classes pre </t>
+  </si>
+  <si>
+    <t>and post query using a naïve look table or a hash table</t>
+  </si>
+  <si>
+    <t>public.bc_ha_slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…\clus\R\digital_elevation_model\01_dem_data_download.R   gdalwarp -r cubic -tap -tr 100 100 -te 159587.5 173787.5 1881187.5 1748187.5 \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\dem\all_bc\slope_all_bc.tif \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\dem\all_bc\bc_slope_prov.tif
+raster2pgsql -s 3005 -d -I -C -M -R \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\dem\all_bc\bc_slope_prov.tif -t 100x100 public.provslope | psql -d clus
+</t>
+  </si>
+  <si>
+    <t>public.veg_comp_lyr_l1_poly</t>
+  </si>
+  <si>
+    <t>ogr2ogr -f PostgreSQL PG:"dbname=clus port = 5432 user=postgres" Z:\FOR\VIC\HTS\FAIB_DATA_FOR_DISTRIBUTION\THLB\2018_BC_THLB\THLB.gdb BC_THLB -overwrite -progress --config PG_USE_COPY YES -nlt PROMOTE_TO_MULTI</t>
   </si>
 </sst>
 </file>
@@ -773,10 +805,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -785,27 +817,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -957,6 +968,27 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
@@ -982,24 +1014,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K43" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K44" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <sortState ref="A2:K43">
     <sortCondition ref="A2:A43"/>
     <sortCondition ref="B2:B43"/>
     <sortCondition ref="G2:G43"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="12" name="Category" dataDxfId="12"/>
-    <tableColumn id="1" name="Information Requirement" dataDxfId="11"/>
-    <tableColumn id="2" name="What is it" dataDxfId="10"/>
-    <tableColumn id="3" name="Uses" dataDxfId="9"/>
-    <tableColumn id="4" name="Dynamic in Simulator?" dataDxfId="8"/>
-    <tableColumn id="5" name="Where is it?" dataDxfId="7"/>
-    <tableColumn id="6" name="Status" dataDxfId="6"/>
-    <tableColumn id="7" name="In postgres db?" dataDxfId="5"/>
-    <tableColumn id="8" name="Spatial extent?" dataDxfId="4"/>
-    <tableColumn id="9" name="Name in postgres db" dataDxfId="3"/>
-    <tableColumn id="13" name="Code" dataDxfId="2"/>
+    <tableColumn id="12" name="Category" dataDxfId="10"/>
+    <tableColumn id="1" name="Information Requirement" dataDxfId="9"/>
+    <tableColumn id="2" name="What is it" dataDxfId="8"/>
+    <tableColumn id="3" name="Uses" dataDxfId="7"/>
+    <tableColumn id="4" name="Dynamic in Simulator?" dataDxfId="6"/>
+    <tableColumn id="5" name="Where is it?" dataDxfId="5"/>
+    <tableColumn id="6" name="Status" dataDxfId="4"/>
+    <tableColumn id="7" name="In postgres db?" dataDxfId="3"/>
+    <tableColumn id="8" name="Spatial extent?" dataDxfId="2"/>
+    <tableColumn id="9" name="Name in postgres db" dataDxfId="1"/>
+    <tableColumn id="13" name="Code" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1295,12 +1327,12 @@
   <sheetPr codeName="Sheet1">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="A7:XFD7"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -1320,7 +1352,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="37" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>36</v>
@@ -1347,30 +1379,30 @@
         <v>35</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="E2" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>3</v>
@@ -1382,27 +1414,27 @@
         <v>12</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>104</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>124</v>
+      <c r="F3" s="11" t="s">
+        <v>123</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>3</v>
@@ -1414,27 +1446,27 @@
         <v>12</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="92.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>96</v>
@@ -1446,30 +1478,30 @@
         <v>12</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="129.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>96</v>
@@ -1481,30 +1513,30 @@
         <v>12</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="E6" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>3</v>
@@ -1516,15 +1548,15 @@
         <v>4</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>9</v>
@@ -1545,15 +1577,21 @@
         <v>3</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>13</v>
@@ -1582,7 +1620,7 @@
     </row>
     <row r="9" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>15</v>
@@ -1611,18 +1649,21 @@
     </row>
     <row r="10" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="C10" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="D10" s="6" t="s">
         <v>97</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -1637,7 +1678,7 @@
     </row>
     <row r="11" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -1666,7 +1707,7 @@
     </row>
     <row r="12" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>84</v>
@@ -1692,10 +1733,16 @@
       <c r="I12" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J12" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>70</v>
@@ -1721,10 +1768,16 @@
       <c r="I13" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="111" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>49</v>
@@ -1750,10 +1803,16 @@
       <c r="I14" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>76</v>
@@ -1782,7 +1841,7 @@
     </row>
     <row r="16" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>78</v>
@@ -1811,7 +1870,7 @@
     </row>
     <row r="17" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>68</v>
@@ -1840,7 +1899,7 @@
     </row>
     <row r="18" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>80</v>
@@ -1869,7 +1928,7 @@
     </row>
     <row r="19" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>74</v>
@@ -1898,7 +1957,7 @@
     </row>
     <row r="20" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>65</v>
@@ -1927,7 +1986,7 @@
     </row>
     <row r="21" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>66</v>
@@ -1956,7 +2015,7 @@
     </row>
     <row r="22" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>67</v>
@@ -1985,7 +2044,7 @@
     </row>
     <row r="23" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>88</v>
@@ -2014,7 +2073,7 @@
     </row>
     <row r="24" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>82</v>
@@ -2043,7 +2102,7 @@
     </row>
     <row r="25" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>82</v>
@@ -2072,16 +2131,16 @@
     </row>
     <row r="26" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>168</v>
-      </c>
       <c r="C26" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>53</v>
@@ -2090,7 +2149,7 @@
         <v>23</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>55</v>
@@ -2103,16 +2162,16 @@
     </row>
     <row r="27" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>53</v>
@@ -2121,7 +2180,7 @@
         <v>23</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>55</v>
@@ -2134,10 +2193,10 @@
     </row>
     <row r="28" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>32</v>
@@ -2163,7 +2222,7 @@
     </row>
     <row r="29" spans="1:11" ht="74" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>5</v>
@@ -2190,12 +2249,12 @@
         <v>4</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>30</v>
@@ -2224,7 +2283,7 @@
     </row>
     <row r="31" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>26</v>
@@ -2253,13 +2312,13 @@
     </row>
     <row r="32" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>39</v>
@@ -2282,7 +2341,7 @@
     </row>
     <row r="33" spans="1:11" ht="74" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>0</v>
@@ -2309,30 +2368,30 @@
         <v>4</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>2</v>
@@ -2344,15 +2403,15 @@
         <v>4</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>24</v>
@@ -2381,22 +2440,22 @@
     </row>
     <row r="36" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
@@ -2408,7 +2467,7 @@
     </row>
     <row r="37" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>28</v>
@@ -2437,7 +2496,7 @@
     </row>
     <row r="38" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>63</v>
@@ -2466,10 +2525,10 @@
     </row>
     <row r="39" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>95</v>
@@ -2481,7 +2540,7 @@
         <v>55</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>96</v>
@@ -2495,22 +2554,22 @@
     </row>
     <row r="40" spans="1:11" ht="37" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>95</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>53</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>96</v>
@@ -2522,12 +2581,12 @@
         <v>12</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>60</v>
@@ -2556,13 +2615,13 @@
     </row>
     <row r="42" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>90</v>
@@ -2574,7 +2633,7 @@
         <v>18</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>55</v>
@@ -2583,18 +2642,18 @@
         <v>12</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="55.5" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="74" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>90</v>
@@ -2603,10 +2662,10 @@
         <v>55</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>55</v>
@@ -2614,9 +2673,25 @@
       <c r="I43" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J43" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="K43" s="6" t="s">
-        <v>154</v>
-      </c>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" s="9"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2624,10 +2699,11 @@
     <hyperlink ref="F29" r:id="rId2"/>
     <hyperlink ref="F10" r:id="rId3"/>
     <hyperlink ref="F4" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2654,10 +2730,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2667,31 +2743,46 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
-      </c>
-      <c r="B1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
red highlighted data that we may not need
</commit_message>
<xml_diff>
--- a/list_clus_data.xlsx
+++ b/list_clus_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="5730"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20700" windowHeight="5730"/>
   </bookViews>
   <sheets>
     <sheet name="Table_Info" sheetId="1" r:id="rId1"/>
@@ -922,7 +922,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -944,6 +944,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1042,6 +1048,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1562,10 +1578,10 @@
   </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2164,34 +2180,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:11" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="H20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -2425,63 +2443,67 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:11" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="H29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" spans="1:11" s="19" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F30" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G30" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="H30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
     </row>
     <row r="31" spans="1:11" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">

</xml_diff>

<commit_message>
updted with wetlands data for boreal BC
</commit_message>
<xml_diff>
--- a/list_clus_data.xlsx
+++ b/list_clus_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="253">
   <si>
     <t>Complete</t>
   </si>
@@ -610,16 +610,6 @@
     <t>All 1ha or greater waterbodies in the province.</t>
   </si>
   <si>
-    <t>Tyler has rasterzied to 1 ha a. In Tyler's postgres or tiffs in \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\water</t>
-  </si>
-  <si>
-    <t>Ducks Unlimited has data for boreal.
-Other areas - use VRI wetland class</t>
-  </si>
-  <si>
-    <t>Need to obtain data.</t>
-  </si>
-  <si>
     <t>Wildlife</t>
   </si>
   <si>
@@ -735,10 +725,6 @@
     <t>Province (most of it…)</t>
   </si>
   <si>
-    <t>Ducks unlimited boreal wetland map (BC in process of purchasing; follow-up with Joelle Scheck in fall/winter). 
-Otherwise use VRI.</t>
-  </si>
-  <si>
     <t>Boreal
 Province</t>
   </si>
@@ -861,6 +847,24 @@
   <si>
     <t>Rasterized to 1ha resolution:
 \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\ski</t>
+  </si>
+  <si>
+    <t>Caribou wetland habitat map derived from a Ducks Unlimited boreal wetland map (see: Wilson and Demars 2015 pdf in CLUS data). 
+Otherwise use VRI.</t>
+  </si>
+  <si>
+    <t>A simpiified classifation specific to cariobu habitat was produced from the Ducks Unlimited data for boreal. The data is downloadable from Hectares BC: https://hectaresbc.ca/app/habc/HaBC.html. 
+Click on the 'raster data' tab, click on the 'enhanced wetland classification' in the data layer window. Click the export raster data button (looks like a sheet of paper with an arrow) and you will be prompted to enter your email and format you want; the data arrives via an email link 
+For other areas - use VRI wetland class</t>
+  </si>
+  <si>
+    <t>Tyler has rasterzied to 1 ha. In Tyler's postgres or tiffs in \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\water</t>
+  </si>
+  <si>
+    <t>In Tyler's postgres or tiffs in \\spatialfiles2.bcgov\archive\FOR\VIC\HTS\ANA\PROJECTS\CLUS\Data\wetland\boreal\Enhanced_Wetland_Classification</t>
+  </si>
+  <si>
+    <t>wetlands_boreal_caribou</t>
   </si>
 </sst>
 </file>
@@ -1578,10 +1582,10 @@
   </sheetPr>
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1768,7 +1772,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="36.950000000000003" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>97</v>
       </c>
@@ -1852,7 +1856,7 @@
         <v>8</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>46</v>
@@ -1881,7 +1885,7 @@
         <v>14</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1939,7 +1943,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>181</v>
+        <v>250</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>46</v>
@@ -1948,7 +1952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="131.25" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>94</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>80</v>
@@ -1965,16 +1969,19 @@
         <v>46</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>183</v>
+        <v>251</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2572,10 +2579,10 @@
         <v>91</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>37</v>
@@ -2584,10 +2591,10 @@
         <v>46</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="H33" s="16" t="s">
         <v>46</v>
@@ -2615,10 +2622,10 @@
         <v>19</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>46</v>
@@ -2647,7 +2654,7 @@
         <v>4</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>45</v>
@@ -2676,10 +2683,10 @@
         <v>83</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>46</v>
@@ -2705,10 +2712,10 @@
         <v>82</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>46</v>
@@ -2725,7 +2732,7 @@
         <v>142</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>34</v>
@@ -2734,10 +2741,10 @@
         <v>46</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H38" s="7" t="s">
         <v>46</v>
@@ -2753,10 +2760,10 @@
         <v>91</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>34</v>
@@ -2765,10 +2772,10 @@
         <v>45</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>45</v>
@@ -2803,7 +2810,7 @@
         <v>120</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>45</v>
@@ -2835,10 +2842,10 @@
         <v>82</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>46</v>
@@ -2852,10 +2859,10 @@
         <v>91</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>81</v>
@@ -2864,10 +2871,10 @@
         <v>46</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H42" s="14" t="s">
         <v>46</v>
@@ -2912,10 +2919,10 @@
         <v>91</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>81</v>
@@ -2924,10 +2931,10 @@
         <v>74</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H44" s="16" t="s">
         <v>46</v>
@@ -2955,10 +2962,10 @@
         <v>82</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>46</v>
@@ -2972,10 +2979,10 @@
         <v>95</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>39</v>
@@ -2984,10 +2991,10 @@
         <v>45</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>46</v>
@@ -3016,7 +3023,7 @@
         <v>115</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>46</v>
@@ -3045,7 +3052,7 @@
         <v>114</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>45</v>
@@ -3106,13 +3113,13 @@
         <v>15</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K50" s="6" t="s">
         <v>134</v>
@@ -3138,13 +3145,13 @@
         <v>133</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K51" s="6" t="s">
         <v>134</v>
@@ -3155,13 +3162,13 @@
         <v>96</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>46</v>
@@ -3170,69 +3177,69 @@
         <v>133</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>46</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J52" s="14"/>
       <c r="K52" s="14"/>
     </row>
     <row r="53" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D53" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="E53" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>200</v>
-      </c>
       <c r="H53" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
     <row r="54" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>193</v>
-      </c>
       <c r="D54" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>46</v>
@@ -3245,25 +3252,25 @@
     </row>
     <row r="55" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H55" s="16" t="s">
         <v>46</v>
@@ -3276,25 +3283,25 @@
     </row>
     <row r="56" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H56" s="16" t="s">
         <v>46</v>
@@ -3307,25 +3314,25 @@
     </row>
     <row r="57" spans="1:11" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>198</v>
-      </c>
       <c r="E57" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H57" s="16" t="s">
         <v>46</v>
@@ -3338,31 +3345,31 @@
     </row>
     <row r="58" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="B58" s="16" t="s">
-        <v>187</v>
-      </c>
       <c r="C58" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H58" s="16" t="s">
         <v>46</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J58" s="16"/>
       <c r="K58" s="16"/>

</xml_diff>